<commit_message>
qpsk 2400 rx wip
</commit_message>
<xml_diff>
--- a/1200_iir_llpf_calc.xlsx
+++ b/1200_iir_llpf_calc.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4102737-285B-B14D-A1D1-15190EC12C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
@@ -19,9 +13,9 @@
     <sheet name="2nd order LPFz" sheetId="1" r:id="rId4"/>
     <sheet name="LFz" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -192,8 +186,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -304,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -356,7 +350,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -550,74 +544,74 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>28800</v>
+        <v>14400</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <f>2*PI()*B2</f>
-        <v>628.31853071795865</v>
+        <v>314.15926535897933</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <f>1/B3</f>
-        <v>3.4722222222222222E-5</v>
+        <v>6.9444444444444444E-5</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -626,13 +620,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>628.34345335856813</v>
+        <v>314.17172667928406</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -641,7 +635,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -653,7 +647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -662,7 +656,7 @@
         <v>2.0218174810193945</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -671,7 +665,7 @@
         <v>1.9781825189806053</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -683,7 +677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -695,7 +689,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -707,15 +701,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>36</v>
       </c>
       <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -723,7 +717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -732,31 +726,31 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20">
         <f>ROUND(B19*B13*B16,0)</f>
-        <v>354</v>
+        <v>2829</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21">
         <f>ROUND(B19*B14*B16,0)</f>
-        <v>354</v>
+        <v>2829</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -777,79 +771,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0218B47B-13FF-3F43-B902-FE92EE5440FF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4800</v>
+        <v>1200</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>28800</v>
+        <v>14400</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <f>2*PI()*B2</f>
-        <v>30159.289474462013</v>
+        <v>7539.8223686155034</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <f>1/B3</f>
-        <v>3.4722222222222222E-5</v>
+        <v>6.9444444444444444E-5</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -858,13 +852,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>33255.375505322438</v>
+        <v>7716.9367420163335</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -873,87 +867,87 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
         <f>B6*B5</f>
-        <v>1.1547005383792512</v>
+        <v>0.53589838486224539</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
         <f>2+(B8)</f>
-        <v>3.1547005383792515</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.5358983848622456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
         <f>2-B8</f>
-        <v>0.84529946162074876</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.4641016151377546</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <f>B10/B9</f>
-        <v>0.26794919243112281</v>
+        <v>0.57735026918962573</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13">
         <f>B8/B9</f>
-        <v>0.36602540378443854</v>
+        <v>0.21132486540518708</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <f>B8/B9</f>
-        <v>0.36602540378443854</v>
+        <v>0.21132486540518708</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>36</v>
       </c>
       <c r="B18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -961,7 +955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -970,49 +964,49 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <f>ROUND(B21*B13*B18,0)</f>
-        <v>23988</v>
+        <v>6925</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <f>ROUND(B21*B14*B18,0)</f>
-        <v>23988</v>
+        <v>6925</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <f>ROUND(B21*B12,0)</f>
-        <v>8780</v>
+        <v>18919</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1020,67 +1014,67 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>37</v>
       </c>
       <c r="B29">
         <f>B13*B13</f>
-        <v>0.13397459621556126</v>
+        <v>4.4658198738520435E-2</v>
       </c>
       <c r="D29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>38</v>
       </c>
       <c r="B30">
         <f>2*B13*B14</f>
-        <v>0.26794919243112253</v>
+        <v>8.9316397477040871E-2</v>
       </c>
       <c r="D30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>39</v>
       </c>
       <c r="B31">
         <f>B14*B14</f>
-        <v>0.13397459621556126</v>
+        <v>4.4658198738520435E-2</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>42</v>
       </c>
       <c r="B33">
         <f>2*B12</f>
-        <v>0.53589838486224561</v>
+        <v>1.1547005383792515</v>
       </c>
       <c r="D33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>43</v>
       </c>
       <c r="B34">
         <f>-B12*B12</f>
-        <v>-7.179676972449088E-2</v>
+        <v>-0.33333333333333331</v>
       </c>
       <c r="D34" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1088,7 +1082,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1097,61 +1091,61 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>44</v>
       </c>
       <c r="B38">
         <f>ROUND(B29*B27*B37,0)</f>
-        <v>4390</v>
+        <v>1463</v>
       </c>
       <c r="D38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>45</v>
       </c>
       <c r="B39">
         <f>ROUND(B30*B27*B37,0)</f>
-        <v>8780</v>
+        <v>2927</v>
       </c>
       <c r="D39" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>46</v>
       </c>
       <c r="B40">
         <f>ROUND(B31*B27*B37,0)</f>
-        <v>4390</v>
+        <v>1463</v>
       </c>
       <c r="D40" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>47</v>
       </c>
       <c r="B41">
         <f>ROUND(B33*B37,0)</f>
-        <v>8780</v>
+        <v>18919</v>
       </c>
       <c r="D41" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>48</v>
       </c>
       <c r="B42">
         <f>ROUND(B34*B37,0)</f>
-        <v>-1176</v>
+        <v>-5461</v>
       </c>
       <c r="D42" t="s">
         <v>20</v>
@@ -1168,27 +1162,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1210,7 +1204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1222,7 +1216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1237,7 +1231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1252,7 +1246,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1264,7 +1258,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1273,7 +1267,7 @@
         <v>2.3078294421196581</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1282,7 +1276,7 @@
         <v>1.6921705578803419</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="17.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1293,7 +1287,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="17.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1301,7 +1295,7 @@
         <v>0.64930619341182005</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1313,7 +1307,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1325,7 +1319,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1334,7 +1328,7 @@
         <v>1.9083729945233441E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1342,7 +1336,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1351,7 +1345,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1363,7 +1357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1375,7 +1369,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1384,7 +1378,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1396,7 +1390,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1414,28 +1408,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1457,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1469,7 +1463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1484,7 +1478,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1499,7 +1493,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1511,7 +1505,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1520,7 +1514,7 @@
         <v>2.0218174810193945</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1529,7 +1523,7 @@
         <v>-1.9781825189806053</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1544,7 +1538,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>B11*1000000</f>
         <v>795.74315181839233</v>
@@ -1553,7 +1547,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1564,7 +1558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1576,7 +1570,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1588,7 +1582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1596,7 +1590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1605,7 +1599,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1617,7 +1611,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1629,7 +1623,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1641,7 +1635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
adj bpsk 1200 tune
</commit_message>
<xml_diff>
--- a/1200_iir_llpf_calc.xlsx
+++ b/1200_iir_llpf_calc.xlsx
@@ -1,25 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F79BAD-37A3-3949-AE17-28948ED33357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
     <sheet name="Branch LPF" sheetId="3" r:id="rId2"/>
     <sheet name="Gains" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -136,8 +130,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -250,7 +244,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -302,7 +296,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -496,34 +490,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -534,7 +528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -545,7 +539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -557,7 +551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -572,7 +566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -587,7 +581,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -599,7 +593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -608,7 +602,7 @@
         <v>2.0436401552442991</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -617,7 +611,7 @@
         <v>1.9563598447557011</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -629,7 +623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -641,7 +635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -653,15 +647,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -669,7 +663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -678,31 +672,31 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1">
         <f>ROUND(B19*B13*B16,0)</f>
-        <v>5598</v>
+        <v>700</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1">
         <f>ROUND(B19*B14*B16,0)</f>
-        <v>5598</v>
+        <v>700</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -723,27 +717,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -754,7 +748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -765,7 +759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -777,7 +771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -792,7 +786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -807,7 +801,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -819,7 +813,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -828,7 +822,7 @@
         <v>2.5358983848622456</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -837,7 +831,7 @@
         <v>1.4641016151377546</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -849,7 +843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -861,7 +855,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -873,21 +867,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -895,7 +889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -904,31 +898,31 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="1">
         <f>ROUND(B21*B13*B18,0)</f>
-        <v>6925</v>
+        <v>27699</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="1">
         <f>ROUND(B21*B14*B18,0)</f>
-        <v>6925</v>
+        <v>27699</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -950,37 +944,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D60D94-7E12-A446-9E46-FB357D1AFF2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
       <c r="B1">
         <f>'LoopFilter LPF'!B16</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
       <c r="B2">
         <f>'Branch LPF'!B18</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -988,13 +982,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4">
         <f>B1*B2*B3</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gain tuning for psk
</commit_message>
<xml_diff>
--- a/1200_iir_llpf_calc.xlsx
+++ b/1200_iir_llpf_calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
@@ -490,7 +490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -720,7 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>

</xml_diff>